<commit_message>
Simulação Monte Carlo para a Kumaraswamy
</commit_message>
<xml_diff>
--- a/kumaraswamy_defective/simulacao_MC_Kumaraswamy.xlsx
+++ b/kumaraswamy_defective/simulacao_MC_Kumaraswamy.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statphd-my.sharepoint.com/personal/dionisioneto_statphd_onmicrosoft_com/Documents/Doutorado em Estatística/2024.2/2_Topicos_Avancados_de_Pesquisa_I/R_code/kumaraswamy_defective/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{160CB99D-0CA4-4BD3-8661-086CE90E97AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{160CB99D-0CA4-4BD3-8661-086CE90E97AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF9E8DA7-7E27-4837-97CA-C4E226DEE9FD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FEEAEB7C-79C1-4F82-8B30-C4F9A8AD2E63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEEAEB7C-79C1-4F82-8B30-C4F9A8AD2E63}"/>
   </bookViews>
   <sheets>
     <sheet name="K_Gompertz_v1" sheetId="1" r:id="rId1"/>
+    <sheet name="K_Inversa_Gaussiana_V1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="28">
   <si>
     <t>N</t>
   </si>
@@ -90,6 +91,36 @@
   </si>
   <si>
     <t>10,000</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>psi ~ gamma(0.25,0.25)</t>
+  </si>
+  <si>
+    <t>kappa ~ gamma(0.25,0.25);</t>
+  </si>
+  <si>
+    <t>beta ~ gamma(0.25,0.25);</t>
+  </si>
+  <si>
+    <t>alpha ~ normal(-1,10);</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>-0.20</t>
+  </si>
+  <si>
+    <t>2.2</t>
   </si>
 </sst>
 </file>
@@ -154,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -162,8 +193,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,14 +212,25 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -199,6 +248,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5877713-1C40-4948-B0FC-80C069D28B56}">
-  <dimension ref="B2:L50"/>
+  <dimension ref="B2:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E3" sqref="E3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,10 +615,10 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="3">
+      <c r="B3" s="15">
         <v>50</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="7">
         <v>0.15</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -583,8 +636,8 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
@@ -600,13 +653,13 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2">
-        <v>2</v>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -617,570 +670,945 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="3">
-        <v>50</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="13"/>
+      <c r="C7" s="7">
         <v>0.45</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="5">
+        <v>-1</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
-        <v>50</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.75</v>
+      <c r="B11" s="15">
+        <v>100</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.15</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>-2</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>10</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="3"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="E14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
-        <v>100</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.15</v>
+      <c r="B15" s="13"/>
+      <c r="C15" s="7">
+        <v>0.45</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="5">
+        <v>-1</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="3">
-        <v>100</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.45</v>
+      <c r="B19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.15</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2">
+        <v>-2</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>10</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="E22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="3">
-        <v>100</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.75</v>
+      <c r="B23" s="12"/>
+      <c r="C23" s="7">
+        <v>0.45</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="5">
+        <v>-1</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="3"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-      <c r="C25" s="5"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="3"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="4">
+      <c r="B27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="7">
         <v>0.15</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="E27" s="2">
+        <v>-2</v>
+      </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="E28" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="E29" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="3"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
+      <c r="E30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="4">
+      <c r="B31" s="10"/>
+      <c r="C31" s="8">
         <v>0.45</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="E31" s="5">
+        <v>-1</v>
+      </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="3"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="7" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="8" t="s">
+      <c r="E34" s="3">
+        <v>2</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="B27:B34"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B18"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAAA4DF-81AD-4FDC-8D7A-0524B0B9AFF3}">
+  <dimension ref="B2:L34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="15">
+        <v>50</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="13"/>
+      <c r="C7" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="13"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="13"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="13">
+        <v>100</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="13"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="13"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="13"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="13"/>
+      <c r="C15" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="13"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="14"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="C19" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="3"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="2" t="s">
+      <c r="E19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="3"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="2" t="s">
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="3"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7" t="s">
+      <c r="E21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="8" t="s">
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="2">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C27" s="7">
         <v>0.15</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="3"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="2" t="s">
+      <c r="E27" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="10"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="3"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="2" t="s">
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7" t="s">
+      <c r="E29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="5">
+      <c r="E30" s="3">
+        <v>2</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="10"/>
+      <c r="C31" s="8">
         <v>0.45</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="3"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="2" t="s">
+      <c r="E31" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="10"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="3"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="2" t="s">
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="10"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7" t="s">
+      <c r="E33" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="8"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="8"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="10"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
+      <c r="E34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="B11:B14"/>
+  <mergeCells count="12">
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B3:B10"/>
     <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B15:B18"/>
     <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B11:B18"/>
     <mergeCell ref="C19:C22"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="B19:B26"/>
     <mergeCell ref="C27:C30"/>
-    <mergeCell ref="B31:B34"/>
     <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B27:B34"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
modelo com covariaveis (freq/bayes) pronto
</commit_message>
<xml_diff>
--- a/kumaraswamy_defective/simulacao_MC_Kumaraswamy.xlsx
+++ b/kumaraswamy_defective/simulacao_MC_Kumaraswamy.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statphd-my.sharepoint.com/personal/dionisioneto_statphd_onmicrosoft_com/Documents/Doutorado em Estatística/2024.2/2_Topicos_Avancados_de_Pesquisa_I/R_code/kumaraswamy_defective/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{160CB99D-0CA4-4BD3-8661-086CE90E97AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF9E8DA7-7E27-4837-97CA-C4E226DEE9FD}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{160CB99D-0CA4-4BD3-8661-086CE90E97AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{506EDC01-1097-488B-8F90-3DDB16AF92A7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FEEAEB7C-79C1-4F82-8B30-C4F9A8AD2E63}"/>
   </bookViews>
   <sheets>
     <sheet name="K_Gompertz_v1" sheetId="1" r:id="rId1"/>
     <sheet name="K_Inversa_Gaussiana_V1" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="37">
   <si>
     <t>N</t>
   </si>
@@ -69,9 +70,6 @@
     <t>$\alpha$</t>
   </si>
   <si>
-    <t>Alpha ~ Normal(0,10^2)</t>
-  </si>
-  <si>
     <t>$\beta$</t>
   </si>
   <si>
@@ -81,9 +79,6 @@
     <t>$\psi$</t>
   </si>
   <si>
-    <t>lambda ~ Gamma(0.001, 0.001)</t>
-  </si>
-  <si>
     <t>$\kappa$</t>
   </si>
   <si>
@@ -121,16 +116,63 @@
   </si>
   <si>
     <t>2.2</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P2 6</t>
+  </si>
+  <si>
+    <t>P2 7</t>
+  </si>
+  <si>
+    <t>P2 8</t>
+  </si>
+  <si>
+    <t>P2 9</t>
+  </si>
+  <si>
+    <t>P2 10</t>
+  </si>
+  <si>
+    <t>Alpha ~ Normal(-1,10^2)</t>
+  </si>
+  <si>
+    <t>kappa ~ Gamma(0.1, 0.1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,8 +224,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -203,6 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -212,29 +256,27 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -574,7 +616,7 @@
   <dimension ref="B2:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,10 +657,10 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="15">
+      <c r="B3" s="11">
         <v>50</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>0.15</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -632,14 +674,14 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="L3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="13"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
         <v>10</v>
@@ -649,43 +691,46 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="L4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="L5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="7">
+      <c r="B7" s="12"/>
+      <c r="C7" s="8">
         <v>0.45</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -700,10 +745,10 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -714,10 +759,10 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -728,10 +773,10 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3">
         <v>2</v>
@@ -742,10 +787,10 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="15">
+      <c r="B11" s="11">
         <v>100</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <v>0.15</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -760,10 +805,10 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -774,13 +819,13 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -788,13 +833,13 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -802,8 +847,8 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="7">
+      <c r="B15" s="12"/>
+      <c r="C15" s="8">
         <v>0.45</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -818,10 +863,10 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -832,10 +877,10 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -846,10 +891,10 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
@@ -860,10 +905,10 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="8">
         <v>0.15</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -878,10 +923,10 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2">
         <v>10</v>
@@ -892,13 +937,13 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -906,13 +951,13 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -920,8 +965,8 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="7">
+      <c r="B23" s="15"/>
+      <c r="C23" s="8">
         <v>0.45</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -936,10 +981,10 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="8"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -950,10 +995,10 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
@@ -964,10 +1009,10 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="3">
         <v>2</v>
@@ -978,10 +1023,10 @@
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="7">
+      <c r="B27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="8">
         <v>0.15</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -992,33 +1037,33 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
-      <c r="C28" s="8"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
-      <c r="C29" s="8"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="15"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E30" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1026,8 +1071,8 @@
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="10"/>
-      <c r="C31" s="8">
+      <c r="B31" s="15"/>
+      <c r="C31" s="9">
         <v>0.45</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1038,30 +1083,30 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="10"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="11"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E34" s="3">
         <v>2</v>
@@ -1136,31 +1181,31 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="15">
+      <c r="B3" s="11">
         <v>50</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>0.15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="13"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1170,31 +1215,31 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
@@ -1204,12 +1249,12 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="7">
+      <c r="B7" s="12"/>
+      <c r="C7" s="8">
         <v>0.45</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1224,10 +1269,10 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
-      <c r="C8" s="8"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
         <v>10</v>
@@ -1238,13 +1283,13 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1252,13 +1297,13 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1266,17 +1311,17 @@
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>100</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <v>0.15</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1284,10 +1329,10 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -1298,13 +1343,13 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1312,10 +1357,10 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
@@ -1326,8 +1371,8 @@
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-      <c r="C15" s="7">
+      <c r="B15" s="12"/>
+      <c r="C15" s="8">
         <v>0.45</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1342,10 +1387,10 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="13"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2">
         <v>10</v>
@@ -1356,13 +1401,13 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1370,13 +1415,13 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1384,17 +1429,17 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="8">
         <v>0.15</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1402,10 +1447,10 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
@@ -1416,13 +1461,13 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1430,10 +1475,10 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="3">
         <v>2</v>
@@ -1444,8 +1489,8 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="7">
+      <c r="B23" s="15"/>
+      <c r="C23" s="8">
         <v>0.45</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -1460,10 +1505,10 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="8"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="2">
         <v>10</v>
@@ -1474,13 +1519,13 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1488,13 +1533,13 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1502,44 +1547,44 @@
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="7">
+      <c r="B27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="8">
         <v>0.15</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
-      <c r="C28" s="8"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
-      <c r="C29" s="8"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="15"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="10"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E30" s="3">
         <v>2</v>
@@ -1550,8 +1595,8 @@
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="10"/>
-      <c r="C31" s="8">
+      <c r="B31" s="15"/>
+      <c r="C31" s="9">
         <v>0.45</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1562,33 +1607,33 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="10"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="16"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="11"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E34" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1612,4 +1657,240 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FBA2D-A5D7-4C35-AC48-778F5E2F95FB}">
+  <dimension ref="D2:P8"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>4.2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <f>($E$2+G3)/2</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <f>($E$2+$G$3+J3)/3</f>
+        <v>5.0666666666666664</v>
+      </c>
+      <c r="M3">
+        <f>($E$2+$G$4+J3)/3</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="N3">
+        <f>($E$2+$G$5+J3)/3</f>
+        <v>5.7333333333333334</v>
+      </c>
+      <c r="O3">
+        <f>($E$2+$G$6+J3)/3</f>
+        <v>6.0666666666666664</v>
+      </c>
+      <c r="P3">
+        <f>($E$2+$G$7+J3)/3</f>
+        <v>6.3999999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H7" si="0">($E$2+G4)/2</f>
+        <v>5.6</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L8" si="1">($E$2+$G$3+J4)/3</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M8" si="2">($E$2+$G$4+J4)/3</f>
+        <v>5.7333333333333334</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N8" si="3">($E$2+$G$5+J4)/3</f>
+        <v>6.0666666666666664</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O8" si="4">($E$2+$G$6+J4)/3</f>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P7" si="5">($E$2+$G$7+J4)/3</f>
+        <v>6.7333333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>6.1</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>5.7333333333333334</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>6.0666666666666664</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>6.7333333333333334</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="5"/>
+        <v>7.0666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>6.6</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>6.0666666666666664</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>6.7333333333333334</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>7.0666666666666664</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="5"/>
+        <v>7.3999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>7.1</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>6.7333333333333334</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>7.0666666666666664</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="5"/>
+        <v>7.7333333333333334</v>
+      </c>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>6.7333333333333334</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>7.0666666666666664</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>7.7333333333333334</v>
+      </c>
+      <c r="P8">
+        <f>($E$2+$G$7+J8)/3</f>
+        <v>8.0666666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>